<commit_message>
chore(requirements): confuse about requirements
</commit_message>
<xml_diff>
--- a/presentations/pal_tabelle.xlsx
+++ b/presentations/pal_tabelle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuebra.tokuc/workspace/Bachelor_Thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuebra.tokuc/workspace/bachelor-thesis/presentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34A73E4-32A9-CB47-B7FF-4D135EF5B57A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B183760D-F8A2-574D-9FFC-8F401F883FD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{2E5F8CF0-7304-1D4E-B5F5-2C530345BB68}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20440" xr2:uid="{2E5F8CF0-7304-1D4E-B5F5-2C530345BB68}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Gesamtsystem</t>
   </si>
@@ -99,18 +99,6 @@
   </si>
   <si>
     <t>K-QA-4: System muss sicher sein</t>
-  </si>
-  <si>
-    <t>Anforderung: Deren Integrität sowie Verfügbarkeit soll gewahrt werden. Daher sollte die Struktur der</t>
-  </si>
-  <si>
-    <t>Verwaltungsschale (Abbildung 3) von Beginn an Aspekten wie Zugriffsschutz, Sichtbarkeit, Identität- und</t>
-  </si>
-  <si>
-    <t>Rechtemanagement, Vertraulichkeit und Integrität Rechnung tragen können. Wenn die getätigte Risikobeurteilung es</t>
-  </si>
-  <si>
-    <t>erlaubt, kann auch ein Zustand "Keine Security" realisiert werden.</t>
   </si>
   <si>
     <r>
@@ -258,12 +246,42 @@
   <si>
     <t>Verwaltungsschale muss von überall zugänglich sein</t>
   </si>
+  <si>
+    <t>Cloud-Hosting</t>
+  </si>
+  <si>
+    <t>Funktional</t>
+  </si>
+  <si>
+    <t>Qualitativ</t>
+  </si>
+  <si>
+    <t>Randbedingung</t>
+  </si>
+  <si>
+    <t>VW muss verfügbar sein</t>
+  </si>
+  <si>
+    <t>VW muss integer sein</t>
+  </si>
+  <si>
+    <t>Zugriffsschutz, Sichtbarkeit, Identitäts- und Rechtmanagement</t>
+  </si>
+  <si>
+    <t>Industrie-4.0-Komponente (besteht aus physischem Asset und Verwaltungsschale)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I40-Komponente muss schachtelbar sein -&gt; logische Zuordnung von anderen Komponten </t>
+  </si>
+  <si>
+    <t>Einflussfaktor/Quelle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -323,8 +341,29 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,8 +406,29 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -376,11 +436,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -388,6 +466,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,42 +512,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -748,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79281457-08DC-CE40-8436-DBFE1BFA0507}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -763,306 +862,337 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="17">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>9</v>
+      <c r="D2" s="21" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:7" ht="39" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="G4" s="22" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="22" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="18"/>
+      <c r="G5" s="23" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="34">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="G6" s="24" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="17">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="25" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="34">
-      <c r="B12" s="15" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="14" spans="1:7" ht="34">
+      <c r="B14" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17">
+      <c r="B15" s="25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17">
+      <c r="B16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="B18" s="11"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="B19" s="11"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="B20" s="11"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="B21" s="11"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" ht="28">
+      <c r="B22" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="41">
+      <c r="B23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="34">
-      <c r="B13" s="15" t="s">
+      <c r="N23" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" ht="34">
-      <c r="B14" s="15" t="s">
+    </row>
+    <row r="24" spans="1:14" ht="41">
+      <c r="B24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" ht="17">
-      <c r="B15" s="15" t="s">
+    </row>
+    <row r="25" spans="1:14" ht="28">
+      <c r="B25" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="66">
+      <c r="A27" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" ht="28">
-      <c r="B16" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="41">
-      <c r="B17" s="13" t="s">
+    </row>
+    <row r="28" spans="1:14" ht="17">
+      <c r="B28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="17">
+      <c r="B29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="17">
+      <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="41">
-      <c r="B18" s="13" t="s">
+      <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="28">
-      <c r="B19" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="66">
-      <c r="A21" s="14" t="s">
+      <c r="N30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="27">
+      <c r="B31" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="17">
-      <c r="B22" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="17">
-      <c r="B23" s="2" t="s">
+    <row r="32" spans="1:14" ht="17">
+      <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N23" t="s">
+    </row>
+    <row r="33" spans="1:14" ht="51">
+      <c r="B33" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="17">
-      <c r="A24" s="2" t="s">
+    <row r="34" spans="1:14" ht="51">
+      <c r="B34" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="51">
+      <c r="B35" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="41">
+      <c r="B36" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="N36" t="s">
         <v>32</v>
       </c>
-      <c r="N24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="27">
-      <c r="B25" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="17">
-      <c r="B26" s="2" t="s">
+    </row>
+    <row r="37" spans="1:14" ht="85">
+      <c r="A37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="34">
+      <c r="B39" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="51">
-      <c r="B27" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="51">
-      <c r="B28" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="51">
-      <c r="B29" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="41">
-      <c r="B30" s="13" t="s">
+    <row r="41" spans="1:14" ht="17">
+      <c r="B41" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N30" t="s">
+      <c r="G41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="85">
-      <c r="A31" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="34">
-      <c r="B33" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="17">
-      <c r="B35" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G35" t="s">
+    <row r="43" spans="1:14" ht="27">
+      <c r="B43" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="27">
-      <c r="B37" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="1" t="s">
+    <row r="44" spans="1:14">
+      <c r="A44" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="40" spans="1:7" ht="17">
-      <c r="A40" s="10" t="s">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="46" spans="1:14" ht="17">
+      <c r="A46" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-    </row>
-    <row r="46" spans="1:7" ht="17">
-      <c r="A46" s="11" t="s">
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="52" spans="1:4" ht="17">
+      <c r="A52" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-    </row>
-    <row r="47" spans="1:7" ht="17">
-      <c r="A47" s="17" t="s">
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4" ht="17">
+      <c r="A53" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B53" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C53" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="18" t="s">
+      <c r="D53" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="17">
-      <c r="A48" s="10" t="s">
+    <row r="54" spans="1:4" ht="17">
+      <c r="A54" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-    </row>
-    <row r="51" spans="1:4" ht="17">
-      <c r="A51" s="10" t="s">
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+    </row>
+    <row r="57" spans="1:4" ht="17">
+      <c r="A57" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="2" t="s">
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17">
-      <c r="A54" s="10" t="s">
+    <row r="60" spans="1:4" ht="17">
+      <c r="A60" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>